<commit_message>
Robo finalizado com sucesso, conforme as aulas do professor.
</commit_message>
<xml_diff>
--- a/Registro_Identidade/ID/Registro.xlsx
+++ b/Registro_Identidade/ID/Registro.xlsx
@@ -1,118 +1,91 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
-  <x:workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E167D763-DF1C-4B54-ABB8-AE64C3A500BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <x:bookViews>
-    <x:workbookView xWindow="28680" yWindow="-1275" windowWidth="29040" windowHeight="15990" firstSheet="0" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </x:bookViews>
-  <x:sheets>
-    <x:sheet name="PESSOAL" sheetId="1" r:id="rId1"/>
-    <x:sheet name="PROFISSIONAL" sheetId="2" r:id="rId2"/>
-    <x:sheet name="ESTUDANTIL" sheetId="3" r:id="rId3"/>
-  </x:sheets>
-  <x:definedNames/>
-  <x:calcPr calcId="122211"/>
-</x:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F4F0C9-A913-4EBC-AACD-13E2A0B2F1B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="28680" yWindow="-1275" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="PESSOAL" sheetId="1" r:id="rId1"/>
+    <sheet name="PROFISSIONAL" sheetId="2" r:id="rId2"/>
+    <sheet name="ESTUDANTIL" sheetId="3" r:id="rId3"/>
+  </sheets>
+  <calcPr calcId="122211"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <x:si>
-    <x:t>ID</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NOME</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NASCIMENTO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Liliane Santos</x:t>
-  </x:si>
-</x:sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>NOME</t>
+  </si>
+  <si>
+    <t>NASCIMENTO</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
-  <x:numFmts count="1">
-    <x:numFmt numFmtId="0" formatCode=""/>
-  </x:numFmts>
-  <x:fonts count="2" x14ac:knownFonts="1">
-    <x:font>
-      <x:sz val="11"/>
-      <x:color theme="1"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-      <x:scheme val="minor"/>
-    </x:font>
-    <x:font>
-      <x:sz val="11"/>
-      <x:color rgb="FF000000"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-    </x:font>
-  </x:fonts>
-  <x:fills count="2">
-    <x:fill>
-      <x:patternFill patternType="none"/>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="gray125"/>
-    </x:fill>
-  </x:fills>
-  <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
-    </x:border>
-  </x:borders>
-  <x:cellStyleXfs count="4">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="14" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-  </x:cellStyleXfs>
-  <x:cellXfs count="6">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-  </x:cellXfs>
-  <x:cellStyles count="1">
-    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </x:cellStyles>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </x:ext>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </x:ext>
-  </x:extLst>
-</x:styleSheet>
+    </ext>
+  </extLst>
+</styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -435,134 +408,97 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1:D3"/>
-  <x:sheetViews>
-    <x:sheetView workbookViewId="0">
-      <x:selection activeCell="A2" sqref="A2 A2:A2 A2:XFD3"/>
-    </x:sheetView>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <x:cols>
-    <x:col min="1" max="2" width="28.140625" style="3" customWidth="1"/>
-    <x:col min="3" max="3" width="13.855469" style="3" bestFit="1" customWidth="1"/>
-    <x:col min="4" max="4" width="10.710938" style="3" bestFit="1" customWidth="1"/>
-  </x:cols>
-  <x:sheetData>
-    <x:row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="3" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="3" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C1" s="3" t="s">
-        <x:v>2</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="3" t="n">
-        <x:v>123956789</x:v>
-      </x:c>
-      <x:c r="B2" s="3" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="C2" s="5">
-        <x:v>31569</x:v>
-      </x:c>
-      <x:c r="D2" s="4" t="s"/>
-    </x:row>
-    <x:row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="D3" s="4" t="s"/>
-    </x:row>
-  </x:sheetData>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="28.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0100-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1:C1"/>
-  <x:sheetViews>
-    <x:sheetView workbookViewId="0">
-      <x:selection activeCell="D7" sqref="D7 D7:D7"/>
-    </x:sheetView>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <x:cols>
-    <x:col min="1" max="1" width="17.710938" style="3" customWidth="1"/>
-    <x:col min="2" max="2" width="20.285156" style="3" customWidth="1"/>
-    <x:col min="3" max="3" width="39.425781" style="3" customWidth="1"/>
-  </x:cols>
-  <x:sheetData>
-    <x:row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="3" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="3" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C1" s="3" t="s">
-        <x:v>2</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:4"/>
-  </x:sheetData>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7 D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0200-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1:C1"/>
-  <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="A39" sqref="A39 A39:A39"/>
-    </x:sheetView>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <x:cols>
-    <x:col min="1" max="1" width="20.570312" style="3" customWidth="1"/>
-    <x:col min="2" max="2" width="30.570312" style="3" customWidth="1"/>
-    <x:col min="3" max="3" width="27.285156" style="3" customWidth="1"/>
-  </x:cols>
-  <x:sheetData>
-    <x:row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="3" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="3" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C1" s="3" t="s">
-        <x:v>2</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="39" spans="1:3">
-      <x:c r="A39" s="3" t="s"/>
-    </x:row>
-  </x:sheetData>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A39" sqref="A39 A39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Primeiro Commit, porém já funcionando! Robo monitora uma pasta de logs e envia o log por e-mail e em seguida move para outra pasta !
</commit_message>
<xml_diff>
--- a/Registro_Identidade/ID/Registro.xlsx
+++ b/Registro_Identidade/ID/Registro.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F4F0C9-A913-4EBC-AACD-13E2A0B2F1B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F744953-A0B5-4665-8B57-6758FA4F941C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1275" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,19 +32,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -67,10 +61,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,7 +415,7 @@
     <col min="4" max="4" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,9 +425,6 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>